<commit_message>
[REF] Tools refactoring step 9
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_tax.xlsx
+++ b/z0bug_odoo/data/account_tax.xlsx
@@ -1046,13 +1046,13 @@
   </sheetPr>
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
@@ -1319,6 +1319,9 @@
       <c r="D8" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" s="0" t="s">
         <v>17</v>
       </c>
@@ -1345,6 +1348,9 @@
       <c r="D9" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
       </c>
@@ -1803,6 +1809,9 @@
       <c r="D22" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F22" s="0" t="s">
         <v>17</v>
       </c>
@@ -1835,6 +1844,9 @@
       <c r="D23" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F23" s="0" t="s">
         <v>17</v>
       </c>
@@ -1861,6 +1873,9 @@
       <c r="D24" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F24" s="0" t="s">
         <v>17</v>
       </c>
@@ -1893,6 +1908,9 @@
       <c r="D25" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F25" s="0" t="s">
         <v>17</v>
       </c>
@@ -1919,6 +1937,9 @@
       <c r="D26" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F26" s="0" t="s">
         <v>17</v>
       </c>
@@ -1945,6 +1966,9 @@
       <c r="D27" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F27" s="0" t="s">
         <v>17</v>
       </c>
@@ -1971,6 +1995,9 @@
       <c r="D28" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F28" s="0" t="s">
         <v>17</v>
       </c>
@@ -2003,6 +2030,9 @@
       <c r="D29" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F29" s="0" t="s">
         <v>17</v>
       </c>
@@ -2029,6 +2059,9 @@
       <c r="D30" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F30" s="0" t="s">
         <v>17</v>
       </c>
@@ -2055,6 +2088,9 @@
       <c r="D31" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F31" s="0" t="s">
         <v>17</v>
       </c>
@@ -2081,6 +2117,9 @@
       <c r="D32" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F32" s="0" t="s">
         <v>17</v>
       </c>
@@ -2113,6 +2152,9 @@
       <c r="D33" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F33" s="0" t="s">
         <v>17</v>
       </c>
@@ -2139,6 +2181,9 @@
       <c r="D34" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F34" s="0" t="s">
         <v>17</v>
       </c>
@@ -2165,6 +2210,9 @@
       <c r="D35" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F35" s="0" t="s">
         <v>17</v>
       </c>
@@ -2191,6 +2239,9 @@
       <c r="D36" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F36" s="0" t="s">
         <v>17</v>
       </c>
@@ -2217,6 +2268,9 @@
       <c r="D37" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F37" s="0" t="s">
         <v>17</v>
       </c>
@@ -2243,6 +2297,9 @@
       <c r="D38" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F38" s="0" t="s">
         <v>17</v>
       </c>
@@ -2269,6 +2326,9 @@
       <c r="D39" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F39" s="0" t="s">
         <v>17</v>
       </c>
@@ -2295,6 +2355,9 @@
       <c r="D40" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F40" s="0" t="s">
         <v>17</v>
       </c>
@@ -2321,6 +2384,9 @@
       <c r="D41" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F41" s="0" t="s">
         <v>17</v>
       </c>
@@ -2347,6 +2413,9 @@
       <c r="D42" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F42" s="0" t="s">
         <v>17</v>
       </c>
@@ -2373,6 +2442,9 @@
       <c r="D43" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="E43" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F43" s="0" t="s">
         <v>17</v>
       </c>
@@ -2469,6 +2541,9 @@
       <c r="D46" s="0" t="n">
         <v>73</v>
       </c>
+      <c r="E46" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F46" s="0" t="s">
         <v>17</v>
       </c>
@@ -2492,6 +2567,9 @@
       <c r="D47" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="E47" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F47" s="0" t="s">
         <v>17</v>
       </c>
@@ -2515,6 +2593,9 @@
       <c r="D48" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="E48" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F48" s="0" t="s">
         <v>17</v>
       </c>
@@ -2538,6 +2619,9 @@
       <c r="D49" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="E49" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F49" s="0" t="s">
         <v>17</v>
       </c>
@@ -2561,6 +2645,9 @@
       <c r="D50" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="E50" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F50" s="0" t="s">
         <v>17</v>
       </c>
@@ -2584,6 +2671,9 @@
       <c r="D51" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="E51" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F51" s="0" t="s">
         <v>17</v>
       </c>
@@ -2607,6 +2697,9 @@
       <c r="D52" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="E52" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F52" s="0" t="s">
         <v>17</v>
       </c>
@@ -2630,6 +2723,9 @@
       <c r="D53" s="0" t="n">
         <v>86</v>
       </c>
+      <c r="E53" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F53" s="0" t="s">
         <v>17</v>
       </c>
@@ -2653,6 +2749,9 @@
       <c r="D54" s="0" t="n">
         <v>87</v>
       </c>
+      <c r="E54" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F54" s="0" t="s">
         <v>17</v>
       </c>
@@ -2676,6 +2775,9 @@
       <c r="D55" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="E55" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F55" s="0" t="s">
         <v>17</v>
       </c>
@@ -2699,6 +2801,9 @@
       <c r="D56" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="E56" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F56" s="0" t="s">
         <v>17</v>
       </c>
@@ -2721,6 +2826,9 @@
       </c>
       <c r="D57" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
[IMP] New stable features
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_tax.xlsx
+++ b/z0bug_odoo/data/account_tax.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="344">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -82,10 +82,7 @@
     <t xml:space="preserve">sale</t>
   </si>
   <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.coa_260010</t>
+    <t xml:space="preserve">external.260010</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_22a</t>
@@ -100,7 +97,7 @@
     <t xml:space="preserve">purchase</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_153010</t>
+    <t xml:space="preserve">external.153010</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_10v</t>
@@ -121,6 +118,24 @@
     <t xml:space="preserve">IVA 10% da acquisti</t>
   </si>
   <si>
+    <t xml:space="preserve">z0bug.tax_5v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 5% su vendite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.tax_5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 5% da acquisti</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_4v</t>
   </si>
   <si>
@@ -145,7 +160,7 @@
     <t xml:space="preserve">a17a</t>
   </si>
   <si>
-    <t xml:space="preserve">Acq.FC IVA Art.17 DPR633</t>
+    <t xml:space="preserve">Acq. FC IVA Art.17 DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">l10n_it_account_tax_kind.n2_2</t>
@@ -166,10 +181,25 @@
     <t xml:space="preserve">a17c2a</t>
   </si>
   <si>
-    <t xml:space="preserve">N.I. art.17 c.2 DPR633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.coa_153050</t>
+    <t xml:space="preserve">Acq. (RC 22%) N.I. art.17 c.2 DPR633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external.153050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external.aa17c2v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.tax_aa17c2v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa17c2v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. charge art.17 c.2 DPR633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external.260050</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a17c2v</t>
@@ -178,10 +208,7 @@
     <t xml:space="preserve">a17c2v</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. charge art.17 c.2 DPR633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.coa_260050</t>
+    <t xml:space="preserve">Vend. (RC 22%) N.I. art.17 c.2 DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a17c6a</t>
@@ -190,7 +217,7 @@
     <t xml:space="preserve">a17c6a</t>
   </si>
   <si>
-    <t xml:space="preserve">N.I. art.17 c.6 DPR633</t>
+    <t xml:space="preserve">Acq. (RC 22%) N.I. art.17 c.6 DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">l10n_it_account_tax_kind.n6_4</t>
@@ -199,16 +226,25 @@
     <t xml:space="preserve">local</t>
   </si>
   <si>
+    <t xml:space="preserve">external.aa17c6v</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_aa17c6v</t>
   </si>
   <si>
+    <t xml:space="preserve">aa17c6v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. charge art.17c6 DPR633</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a17c6v</t>
   </si>
   <si>
     <t xml:space="preserve">a17c6v</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. charge art.17c6 DPR633</t>
+    <t xml:space="preserve">Vend. (RC 22%) N.I. art.17c6 DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a17c6ata</t>
@@ -217,22 +253,31 @@
     <t xml:space="preserve">a17c6ata</t>
   </si>
   <si>
-    <t xml:space="preserve">N.I. Art.17 c.6 lett. A-ter DPR633</t>
+    <t xml:space="preserve">Acq. (RC 22%) N.I. Art.17 c.6 lett. A-ter DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">l10n_it_account_tax_kind.n6_7</t>
   </si>
   <si>
+    <t xml:space="preserve">external.aa17c6atv</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_aa17c6atv</t>
   </si>
   <si>
+    <t xml:space="preserve">aa17c6atv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. Charge Art.17 c.6 lett. A-ter DPR633</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a17c6atv</t>
   </si>
   <si>
     <t xml:space="preserve">a17c6atv</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. Charge Art.17 c.6 lett. A-ter DPR633</t>
+    <t xml:space="preserve">Vend.(RC 22%) N.I. Art.17 c.6 lett. A-ter DPR633</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a17c6ba</t>
@@ -241,22 +286,34 @@
     <t xml:space="preserve">a17c6ba</t>
   </si>
   <si>
-    <t xml:space="preserve">N.I. art.17 c.6 lett. B DPR633 (Cellulari)</t>
+    <t xml:space="preserve">Acq. (RC 22%) N.I. art.17 c.6 lett. B DPR633 (Cellulari)</t>
   </si>
   <si>
     <t xml:space="preserve">l10n_it_account_tax_kind.n6_5</t>
   </si>
   <si>
+    <t xml:space="preserve">external.aa17c6bv</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_aa17c6bv</t>
   </si>
   <si>
+    <t xml:space="preserve">aa17c6bv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. Charge art.17 c.6 lett. B DPR633 (Cellulari)</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a17c6bv</t>
   </si>
   <si>
     <t xml:space="preserve">a17c6bv</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. Charge art.17 c.6 lett. B DPR633 (Cellulari)</t>
+    <t xml:space="preserve">Vend. (RC 22%) art.17 c.6 lett. B DPR633 (Cellulari)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_it_account_tax_kind.n6_6</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a17c6ca</t>
@@ -265,22 +322,28 @@
     <t xml:space="preserve">a17c6ca</t>
   </si>
   <si>
-    <t xml:space="preserve">N.I. Art.17 c.6 lett. C DPR633 (Elettronici)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_account_tax_kind.n6_6</t>
+    <t xml:space="preserve">Acq. (RC 22%) N.I. Art.17 c.6 lett. C DPR633 (Elettronici)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external.aa17c6cv</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_aa17c6cv</t>
   </si>
   <si>
+    <t xml:space="preserve">aa17c6cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. Charge Art.17 c.6 lett. C DPR633 (Elettronici)</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a17c6cv</t>
   </si>
   <si>
     <t xml:space="preserve">a17c6cv</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. Charge Art.17 c.6 lett. C DPR633 (Elettronici)</t>
+    <t xml:space="preserve">Vend. (RC 22%) Art.17 c.6 lett. C DPR633 (Elettronici)</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a38a</t>
@@ -292,13 +355,37 @@
     <t xml:space="preserve">N.I. art.38 L.427/93</t>
   </si>
   <si>
+    <t xml:space="preserve">external.aa38v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.tax_aa38v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa38v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. charge art.38 L.427/93</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a38v</t>
   </si>
   <si>
     <t xml:space="preserve">a38v</t>
   </si>
   <si>
-    <t xml:space="preserve">Rev. charge art.38 L.427/93</t>
+    <t xml:space="preserve">Vend. N.I. Art.38 L.427/93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.tax_aa41a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa41a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acq.N.I. art.41 L.427/93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_it_account_tax_kind.n3_2</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a41a</t>
@@ -307,13 +394,10 @@
     <t xml:space="preserve">a41a</t>
   </si>
   <si>
-    <t xml:space="preserve">Acq.N.I. art.41 L.427/93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_account_tax_kind.n3_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.tax_aa41v</t>
+    <t xml:space="preserve">Vend.N.I. art.41 L.427/93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external.aa41v</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a41v</t>
@@ -322,9 +406,6 @@
     <t xml:space="preserve">a41v</t>
   </si>
   <si>
-    <t xml:space="preserve">Vend.N.I. art.41 L.427/93</t>
-  </si>
-  <si>
     <t xml:space="preserve">z0bug.tax_a7a</t>
   </si>
   <si>
@@ -340,7 +421,7 @@
     <t xml:space="preserve">self</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.tax_aa7v</t>
+    <t xml:space="preserve">external.aa7v</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a7v</t>
@@ -382,9 +463,18 @@
     <t xml:space="preserve">l10n_it_account_tax_kind.n3_4</t>
   </si>
   <si>
+    <t xml:space="preserve">external.aa8av</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_aa8av</t>
   </si>
   <si>
+    <t xml:space="preserve">aa8av</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev. Charge art.8a DPR633 (Dogana)</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.tax_a8av</t>
   </si>
   <si>
@@ -424,7 +514,7 @@
     <t xml:space="preserve">Acq.N.I. art.9 DPR633</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.tax_aa9v</t>
+    <t xml:space="preserve">external.aa9v</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a9v</t>
@@ -541,7 +631,7 @@
     <t xml:space="preserve">IVA 22% per cassa (art. 32 bis DPR 83/2012) su vendite</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_260030</t>
+    <t xml:space="preserve">external.260030</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -556,7 +646,7 @@
     <t xml:space="preserve">IVA 22% per cassa (art. 32 bis DPR 83/2012) su acquisti</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_153030</t>
+    <t xml:space="preserve">external.153030</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a10c5a</t>
@@ -676,9 +766,6 @@
     <t xml:space="preserve">IVA 22% da scorporare</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">z0bug.tax_10vINC</t>
   </si>
   <si>
@@ -727,7 +814,7 @@
     <t xml:space="preserve">17.6</t>
   </si>
   <si>
-    <t xml:space="preserve">\N</t>
+    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_2250a</t>
@@ -907,54 +994,36 @@
     <t xml:space="preserve">z0bug.tax_2250</t>
   </si>
   <si>
-    <t xml:space="preserve">2250</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 22% detraibile 50%</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_2220</t>
   </si>
   <si>
-    <t xml:space="preserve">2220</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 22% detraibile 20%</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_2280</t>
   </si>
   <si>
-    <t xml:space="preserve">2280</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 22% detraibile 80%</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_2270</t>
   </si>
   <si>
-    <t xml:space="preserve">2270</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 22% detraibile 70%</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_1050</t>
   </si>
   <si>
-    <t xml:space="preserve">1050</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 10% detraibile 50%</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_450</t>
   </si>
   <si>
-    <t xml:space="preserve">450</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 4% detraibile 50%</t>
   </si>
   <si>
@@ -967,7 +1036,7 @@
     <t xml:space="preserve">Art. 17ter - split-payment</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_260060</t>
+    <t xml:space="preserve">external.260060</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
@@ -989,15 +1058,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1063,7 +1132,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1072,8 +1141,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1093,31 +1166,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F95" activeCellId="0" sqref="F95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92:C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,25 +1259,25 @@
       <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -1219,27 +1289,27 @@
         <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3</v>
@@ -1253,25 +1323,25 @@
       <c r="H4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>3</v>
@@ -1283,33 +1353,33 @@
         <v>18</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>18</v>
@@ -1317,155 +1387,149 @@
       <c r="H6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K6" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="K7" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="E8" s="0" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>42</v>
+      <c r="K8" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="E10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="E11" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F11" s="0" t="n">
         <v>22</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -1474,31 +1538,25 @@
       <c r="H11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="E12" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>22</v>
@@ -1507,39 +1565,36 @@
         <v>18</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>26</v>
+        <v>200</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>22</v>
@@ -1550,28 +1605,28 @@
       <c r="H13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>20</v>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>22</v>
@@ -1580,39 +1635,33 @@
         <v>18</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>22</v>
@@ -1621,30 +1670,39 @@
         <v>18</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="E16" s="0" t="n">
-        <v>29</v>
+        <v>200</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>22</v>
@@ -1653,39 +1711,30 @@
         <v>18</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>22</v>
@@ -1696,28 +1745,28 @@
       <c r="H17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>20</v>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>22</v>
@@ -1726,39 +1775,39 @@
         <v>18</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>22</v>
@@ -1769,28 +1818,28 @@
       <c r="H19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>20</v>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>22</v>
@@ -1799,33 +1848,30 @@
         <v>18</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>22</v>
@@ -1834,71 +1880,74 @@
         <v>18</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="E22" s="0" t="n">
-        <v>36</v>
+        <v>200</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>97</v>
+        <v>19</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>18</v>
@@ -1906,63 +1955,78 @@
       <c r="H23" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>20</v>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>42</v>
+        <v>200</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>18</v>
@@ -1970,83 +2034,104 @@
       <c r="H25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>104</v>
+      <c r="I25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>22</v>
@@ -2055,39 +2140,33 @@
         <v>18</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="N28" s="0" t="s">
-        <v>120</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>22</v>
@@ -2098,89 +2177,110 @@
       <c r="H29" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>20</v>
+      <c r="I29" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>47</v>
+        <v>200</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>0</v>
@@ -2189,33 +2289,27 @@
         <v>18</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="N32" s="0" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>0</v>
@@ -2224,27 +2318,33 @@
         <v>18</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>0</v>
@@ -2253,27 +2353,27 @@
         <v>18</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>141</v>
+        <v>19</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>0</v>
@@ -2282,27 +2382,27 @@
         <v>18</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>141</v>
+        <v>24</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>0</v>
@@ -2311,88 +2411,106 @@
         <v>18</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>18</v>
@@ -2400,25 +2518,31 @@
       <c r="H39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="0" t="s">
-        <v>20</v>
+      <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>0</v>
@@ -2427,27 +2551,27 @@
         <v>18</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>0</v>
@@ -2458,54 +2582,60 @@
       <c r="H41" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="0" t="s">
-        <v>20</v>
+      <c r="I41" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="N42" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>69</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="E43" s="0" t="n">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>0</v>
@@ -2514,97 +2644,85 @@
         <v>18</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="E44" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>71</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="O44" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="O45" s="0" t="s">
-        <v>174</v>
+        <v>19</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>0</v>
@@ -2613,24 +2731,27 @@
         <v>18</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>0</v>
@@ -2641,22 +2762,25 @@
       <c r="H47" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I47" s="0" t="s">
-        <v>20</v>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>0</v>
@@ -2665,24 +2789,27 @@
         <v>18</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>0</v>
@@ -2693,22 +2820,25 @@
       <c r="H49" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I49" s="0" t="s">
-        <v>20</v>
+      <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>0</v>
@@ -2717,24 +2847,27 @@
         <v>18</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>0</v>
@@ -2745,22 +2878,25 @@
       <c r="H51" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I51" s="0" t="s">
-        <v>20</v>
+      <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>0</v>
@@ -2769,24 +2905,27 @@
         <v>18</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>0</v>
@@ -2795,62 +2934,83 @@
         <v>18</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="K54" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="O54" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="E54" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="D55" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="E55" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="E55" s="0" t="n">
-        <v>88</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>20</v>
+      <c r="K55" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="O55" s="0" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,7 +3024,7 @@
         <v>211</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>0</v>
@@ -2873,10 +3033,10 @@
         <v>18</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,7 +3050,7 @@
         <v>214</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>0</v>
@@ -2901,8 +3061,8 @@
       <c r="H57" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I57" s="0" t="s">
-        <v>20</v>
+      <c r="I57" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,42 +3076,36 @@
         <v>217</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K58" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="D59" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>221</v>
-      </c>
       <c r="E59" s="0" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>18</v>
@@ -2959,875 +3113,1141 @@
       <c r="H59" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J59" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K59" s="0" t="s">
-        <v>21</v>
+      <c r="I59" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="D60" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>224</v>
-      </c>
       <c r="E60" s="0" t="n">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J60" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K60" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="D61" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>227</v>
-      </c>
       <c r="E61" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="D62" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>230</v>
-      </c>
       <c r="E62" s="0" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="D63" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>233</v>
-      </c>
       <c r="E63" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>234</v>
+        <v>86</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>242</v>
+        <v>88</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>246</v>
+        <v>89</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I68" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I69" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>200</v>
+        <v>93</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I70" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J70" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="K70" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>246</v>
+        <v>100</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J72" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K72" s="0" t="s">
-        <v>26</v>
+      <c r="H72" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>263</v>
       </c>
       <c r="G73" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K73" s="0" t="s">
-        <v>26</v>
+        <v>264</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>271</v>
+        <v>100</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="G74" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K74" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>234</v>
+        <v>271</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="I75" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J75" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K75" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F76" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="E76" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="G76" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I76" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J76" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K76" s="0" t="s">
-        <v>26</v>
+        <v>264</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="C77" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>280</v>
-      </c>
       <c r="E77" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J77" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K77" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D78" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>283</v>
-      </c>
       <c r="E78" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J78" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K78" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="D79" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="C79" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>286</v>
-      </c>
       <c r="E79" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I79" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H80" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I80" s="0" t="s">
-        <v>20</v>
+      <c r="K80" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H81" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I81" s="0" t="s">
-        <v>20</v>
+      <c r="K81" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>22</v>
+        <v>200</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>275</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H82" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I82" s="0" t="s">
-        <v>20</v>
+      <c r="K82" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H83" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I83" s="0" t="s">
-        <v>20</v>
+      <c r="K83" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F84" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="C84" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="E84" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>22</v>
-      </c>
       <c r="G84" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H84" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I84" s="0" t="s">
-        <v>20</v>
+      <c r="K84" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="C85" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>305</v>
-      </c>
       <c r="E85" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>22</v>
+        <v>200</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>263</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H85" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I85" s="0" t="s">
-        <v>20</v>
+      <c r="K85" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="C86" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>308</v>
-      </c>
       <c r="E86" s="0" t="n">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H86" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I86" s="0" t="s">
-        <v>20</v>
+      <c r="K86" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="C87" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>311</v>
-      </c>
       <c r="E87" s="0" t="n">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="H87" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I87" s="0" t="s">
-        <v>20</v>
+      <c r="K87" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="C88" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>314</v>
-      </c>
       <c r="E88" s="0" t="n">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G88" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I88" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>315</v>
+        <v>25</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="O88" s="0" t="s">
-        <v>316</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="C90" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="D90" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="E90" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="E89" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="F89" s="0" t="n">
+      <c r="C91" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="C92" s="3" t="n">
+        <v>2250</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C93" s="3" t="n">
+        <v>2220</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="C94" s="3" t="n">
+        <v>2280</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C95" s="3" t="n">
+        <v>2270</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H95" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="C96" s="3" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I96" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C97" s="3" t="n">
+        <v>450</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I97" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I98" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="K98" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="O98" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F99" s="0" t="n">
         <v>-22</v>
       </c>
-      <c r="G89" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H89" s="0" t="s">
+      <c r="G99" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H99" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I89" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J89" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="K89" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="O89" s="0" t="s">
-        <v>316</v>
+      <c r="I99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="K99" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="O99" s="0" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>